<commit_message>
finished doing regressions for the 0.7 mm
</commit_message>
<xml_diff>
--- a/GSD/baskets_new_sizes/trap_regressions_extra.xlsx
+++ b/GSD/baskets_new_sizes/trap_regressions_extra.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\baskets_new_sizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A505C042-938F-48D2-A155-8B65CBB915D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7B09EE-8F21-43BA-ADBF-04E793219177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{EF1BCDA9-8B94-427C-8470-DDC0752739A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{EF1BCDA9-8B94-427C-8470-DDC0752739A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity vs Deposition" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1472,10 +1472,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1487,10 +1490,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1502,19 +1511,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1523,10 +1523,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1535,10 +1541,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -39309,16 +39312,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>519953</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>29766</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>170330</xdr:rowOff>
+      <xdr:rowOff>170331</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>161365</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>44823</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>160735</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39906,10 +39909,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="202" t="s">
+      <c r="A2" s="204" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="202"/>
+      <c r="B2" s="204"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -40209,10 +40212,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="202"/>
+      <c r="B17" s="204"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -40489,10 +40492,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="202" t="s">
+      <c r="A31" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="202"/>
+      <c r="B31" s="204"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
@@ -40769,10 +40772,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="202" t="s">
+      <c r="A45" s="204" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="202"/>
+      <c r="B45" s="204"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
@@ -41080,74 +41083,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="209" t="s">
+      <c r="A1" s="212" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="210"/>
-      <c r="C1" s="210"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="210"/>
-      <c r="F1" s="210"/>
-      <c r="G1" s="210"/>
-      <c r="H1" s="210"/>
-      <c r="I1" s="210"/>
-      <c r="J1" s="210"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
-      <c r="M1" s="210"/>
-      <c r="N1" s="210"/>
-      <c r="O1" s="210"/>
-      <c r="P1" s="210"/>
-      <c r="Q1" s="211"/>
+      <c r="B1" s="213"/>
+      <c r="C1" s="213"/>
+      <c r="D1" s="213"/>
+      <c r="E1" s="213"/>
+      <c r="F1" s="213"/>
+      <c r="G1" s="213"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="213"/>
+      <c r="K1" s="213"/>
+      <c r="L1" s="213"/>
+      <c r="M1" s="213"/>
+      <c r="N1" s="213"/>
+      <c r="O1" s="213"/>
+      <c r="P1" s="213"/>
+      <c r="Q1" s="214"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
-      <c r="J2" s="208"/>
-      <c r="K2" s="208"/>
-      <c r="L2" s="208"/>
-      <c r="M2" s="208"/>
-      <c r="N2" s="208"/>
-      <c r="O2" s="208"/>
-      <c r="P2" s="208"/>
-      <c r="Q2" s="208"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="I2" s="216"/>
+      <c r="J2" s="216"/>
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="216"/>
+      <c r="N2" s="216"/>
+      <c r="O2" s="216"/>
+      <c r="P2" s="216"/>
+      <c r="Q2" s="216"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="82"/>
-      <c r="B3" s="203" t="s">
+      <c r="B3" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203" t="s">
+      <c r="C3" s="211"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203" t="s">
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="203"/>
-      <c r="J3" s="203"/>
-      <c r="K3" s="203" t="s">
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
+      <c r="K3" s="211" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="203"/>
-      <c r="M3" s="203"/>
-      <c r="N3" s="203" t="s">
+      <c r="L3" s="211"/>
+      <c r="M3" s="211"/>
+      <c r="N3" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="203"/>
-      <c r="P3" s="203"/>
+      <c r="O3" s="211"/>
+      <c r="P3" s="211"/>
       <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -41820,53 +41823,53 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="204" t="s">
+      <c r="A17" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="205"/>
-      <c r="C17" s="205"/>
-      <c r="D17" s="205"/>
-      <c r="E17" s="205"/>
-      <c r="F17" s="205"/>
-      <c r="G17" s="205"/>
-      <c r="H17" s="205"/>
-      <c r="I17" s="205"/>
-      <c r="J17" s="205"/>
-      <c r="K17" s="205"/>
-      <c r="L17" s="205"/>
-      <c r="M17" s="205"/>
-      <c r="N17" s="205"/>
-      <c r="O17" s="205"/>
-      <c r="P17" s="205"/>
-      <c r="Q17" s="206"/>
+      <c r="B17" s="206"/>
+      <c r="C17" s="206"/>
+      <c r="D17" s="206"/>
+      <c r="E17" s="206"/>
+      <c r="F17" s="206"/>
+      <c r="G17" s="206"/>
+      <c r="H17" s="206"/>
+      <c r="I17" s="206"/>
+      <c r="J17" s="206"/>
+      <c r="K17" s="206"/>
+      <c r="L17" s="206"/>
+      <c r="M17" s="206"/>
+      <c r="N17" s="206"/>
+      <c r="O17" s="206"/>
+      <c r="P17" s="206"/>
+      <c r="Q17" s="207"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="82"/>
-      <c r="B18" s="212" t="s">
+      <c r="B18" s="208" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="213"/>
-      <c r="D18" s="214"/>
-      <c r="E18" s="212" t="s">
+      <c r="C18" s="209"/>
+      <c r="D18" s="210"/>
+      <c r="E18" s="208" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="213"/>
-      <c r="G18" s="214"/>
-      <c r="H18" s="212" t="s">
+      <c r="F18" s="209"/>
+      <c r="G18" s="210"/>
+      <c r="H18" s="208" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="213"/>
-      <c r="J18" s="214"/>
-      <c r="K18" s="212" t="s">
+      <c r="I18" s="209"/>
+      <c r="J18" s="210"/>
+      <c r="K18" s="208" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="213"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="203" t="s">
+      <c r="L18" s="209"/>
+      <c r="M18" s="210"/>
+      <c r="N18" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="203"/>
-      <c r="P18" s="203"/>
+      <c r="O18" s="211"/>
+      <c r="P18" s="211"/>
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -42371,74 +42374,74 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="209" t="s">
+      <c r="A46" s="212" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="210"/>
-      <c r="C46" s="210"/>
-      <c r="D46" s="210"/>
-      <c r="E46" s="210"/>
-      <c r="F46" s="210"/>
-      <c r="G46" s="210"/>
-      <c r="H46" s="210"/>
-      <c r="I46" s="210"/>
-      <c r="J46" s="210"/>
-      <c r="K46" s="210"/>
-      <c r="L46" s="210"/>
-      <c r="M46" s="210"/>
-      <c r="N46" s="210"/>
-      <c r="O46" s="210"/>
-      <c r="P46" s="210"/>
-      <c r="Q46" s="211"/>
+      <c r="B46" s="213"/>
+      <c r="C46" s="213"/>
+      <c r="D46" s="213"/>
+      <c r="E46" s="213"/>
+      <c r="F46" s="213"/>
+      <c r="G46" s="213"/>
+      <c r="H46" s="213"/>
+      <c r="I46" s="213"/>
+      <c r="J46" s="213"/>
+      <c r="K46" s="213"/>
+      <c r="L46" s="213"/>
+      <c r="M46" s="213"/>
+      <c r="N46" s="213"/>
+      <c r="O46" s="213"/>
+      <c r="P46" s="213"/>
+      <c r="Q46" s="214"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="207" t="s">
+      <c r="A47" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="208"/>
-      <c r="C47" s="208"/>
-      <c r="D47" s="208"/>
-      <c r="E47" s="208"/>
-      <c r="F47" s="208"/>
-      <c r="G47" s="208"/>
-      <c r="H47" s="208"/>
-      <c r="I47" s="208"/>
-      <c r="J47" s="208"/>
-      <c r="K47" s="208"/>
-      <c r="L47" s="208"/>
-      <c r="M47" s="208"/>
-      <c r="N47" s="208"/>
-      <c r="O47" s="208"/>
-      <c r="P47" s="208"/>
-      <c r="Q47" s="208"/>
+      <c r="B47" s="216"/>
+      <c r="C47" s="216"/>
+      <c r="D47" s="216"/>
+      <c r="E47" s="216"/>
+      <c r="F47" s="216"/>
+      <c r="G47" s="216"/>
+      <c r="H47" s="216"/>
+      <c r="I47" s="216"/>
+      <c r="J47" s="216"/>
+      <c r="K47" s="216"/>
+      <c r="L47" s="216"/>
+      <c r="M47" s="216"/>
+      <c r="N47" s="216"/>
+      <c r="O47" s="216"/>
+      <c r="P47" s="216"/>
+      <c r="Q47" s="216"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="82"/>
-      <c r="B48" s="203" t="s">
+      <c r="B48" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="203"/>
-      <c r="D48" s="203"/>
-      <c r="E48" s="203" t="s">
+      <c r="C48" s="211"/>
+      <c r="D48" s="211"/>
+      <c r="E48" s="211" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="203"/>
-      <c r="G48" s="203"/>
-      <c r="H48" s="203" t="s">
+      <c r="F48" s="211"/>
+      <c r="G48" s="211"/>
+      <c r="H48" s="211" t="s">
         <v>36</v>
       </c>
-      <c r="I48" s="203"/>
-      <c r="J48" s="203"/>
-      <c r="K48" s="203" t="s">
+      <c r="I48" s="211"/>
+      <c r="J48" s="211"/>
+      <c r="K48" s="211" t="s">
         <v>37</v>
       </c>
-      <c r="L48" s="203"/>
-      <c r="M48" s="203"/>
-      <c r="N48" s="203" t="s">
+      <c r="L48" s="211"/>
+      <c r="M48" s="211"/>
+      <c r="N48" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="O48" s="203"/>
-      <c r="P48" s="203"/>
+      <c r="O48" s="211"/>
+      <c r="P48" s="211"/>
       <c r="Q48" s="10"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -43111,53 +43114,53 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62" s="204" t="s">
+      <c r="A62" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="205"/>
-      <c r="C62" s="205"/>
-      <c r="D62" s="205"/>
-      <c r="E62" s="205"/>
-      <c r="F62" s="205"/>
-      <c r="G62" s="205"/>
-      <c r="H62" s="205"/>
-      <c r="I62" s="205"/>
-      <c r="J62" s="205"/>
-      <c r="K62" s="205"/>
-      <c r="L62" s="205"/>
-      <c r="M62" s="205"/>
-      <c r="N62" s="205"/>
-      <c r="O62" s="205"/>
-      <c r="P62" s="205"/>
-      <c r="Q62" s="206"/>
+      <c r="B62" s="206"/>
+      <c r="C62" s="206"/>
+      <c r="D62" s="206"/>
+      <c r="E62" s="206"/>
+      <c r="F62" s="206"/>
+      <c r="G62" s="206"/>
+      <c r="H62" s="206"/>
+      <c r="I62" s="206"/>
+      <c r="J62" s="206"/>
+      <c r="K62" s="206"/>
+      <c r="L62" s="206"/>
+      <c r="M62" s="206"/>
+      <c r="N62" s="206"/>
+      <c r="O62" s="206"/>
+      <c r="P62" s="206"/>
+      <c r="Q62" s="207"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="82"/>
-      <c r="B63" s="212" t="s">
+      <c r="B63" s="208" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="213"/>
-      <c r="D63" s="214"/>
-      <c r="E63" s="212" t="s">
+      <c r="C63" s="209"/>
+      <c r="D63" s="210"/>
+      <c r="E63" s="208" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="213"/>
-      <c r="G63" s="214"/>
-      <c r="H63" s="212" t="s">
+      <c r="F63" s="209"/>
+      <c r="G63" s="210"/>
+      <c r="H63" s="208" t="s">
         <v>36</v>
       </c>
-      <c r="I63" s="213"/>
-      <c r="J63" s="214"/>
-      <c r="K63" s="212" t="s">
+      <c r="I63" s="209"/>
+      <c r="J63" s="210"/>
+      <c r="K63" s="208" t="s">
         <v>37</v>
       </c>
-      <c r="L63" s="213"/>
-      <c r="M63" s="214"/>
-      <c r="N63" s="203" t="s">
+      <c r="L63" s="209"/>
+      <c r="M63" s="210"/>
+      <c r="N63" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="O63" s="203"/>
-      <c r="P63" s="203"/>
+      <c r="O63" s="211"/>
+      <c r="P63" s="211"/>
       <c r="Q63" s="1"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -43663,19 +43666,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A62:Q62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="K63:M63"/>
-    <mergeCell ref="N63:P63"/>
-    <mergeCell ref="A46:Q46"/>
-    <mergeCell ref="A47:Q47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="N48:P48"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="A17:Q17"/>
@@ -43689,6 +43679,19 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
+    <mergeCell ref="A46:Q46"/>
+    <mergeCell ref="A47:Q47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="N48:P48"/>
+    <mergeCell ref="A62:Q62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="K63:M63"/>
+    <mergeCell ref="N63:P63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -43725,40 +43728,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="219" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="216"/>
+      <c r="C1" s="219"/>
       <c r="I1" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="219" t="s">
+      <c r="J1" s="221" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="219"/>
-      <c r="L1" s="215" t="s">
+      <c r="K1" s="221"/>
+      <c r="L1" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="215"/>
-      <c r="O1" s="209" t="s">
+      <c r="M1" s="222"/>
+      <c r="O1" s="212" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="210"/>
-      <c r="Q1" s="210"/>
-      <c r="R1" s="210"/>
-      <c r="S1" s="210"/>
-      <c r="T1" s="210"/>
-      <c r="U1" s="210"/>
-      <c r="V1" s="210"/>
-      <c r="W1" s="210"/>
-      <c r="X1" s="210"/>
-      <c r="Y1" s="210"/>
-      <c r="Z1" s="210"/>
-      <c r="AA1" s="210"/>
-      <c r="AB1" s="210"/>
-      <c r="AC1" s="210"/>
-      <c r="AD1" s="210"/>
-      <c r="AE1" s="211"/>
+      <c r="P1" s="213"/>
+      <c r="Q1" s="213"/>
+      <c r="R1" s="213"/>
+      <c r="S1" s="213"/>
+      <c r="T1" s="213"/>
+      <c r="U1" s="213"/>
+      <c r="V1" s="213"/>
+      <c r="W1" s="213"/>
+      <c r="X1" s="213"/>
+      <c r="Y1" s="213"/>
+      <c r="Z1" s="213"/>
+      <c r="AA1" s="213"/>
+      <c r="AB1" s="213"/>
+      <c r="AC1" s="213"/>
+      <c r="AD1" s="213"/>
+      <c r="AE1" s="214"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -43795,25 +43798,25 @@
       <c r="M2" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="207" t="s">
+      <c r="O2" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="208"/>
-      <c r="Q2" s="208"/>
-      <c r="R2" s="208"/>
-      <c r="S2" s="208"/>
-      <c r="T2" s="208"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="208"/>
-      <c r="W2" s="208"/>
-      <c r="X2" s="208"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="208"/>
-      <c r="AB2" s="208"/>
-      <c r="AC2" s="208"/>
-      <c r="AD2" s="208"/>
-      <c r="AE2" s="208"/>
+      <c r="P2" s="216"/>
+      <c r="Q2" s="216"/>
+      <c r="R2" s="216"/>
+      <c r="S2" s="216"/>
+      <c r="T2" s="216"/>
+      <c r="U2" s="216"/>
+      <c r="V2" s="216"/>
+      <c r="W2" s="216"/>
+      <c r="X2" s="216"/>
+      <c r="Y2" s="216"/>
+      <c r="Z2" s="216"/>
+      <c r="AA2" s="216"/>
+      <c r="AB2" s="216"/>
+      <c r="AC2" s="216"/>
+      <c r="AD2" s="216"/>
+      <c r="AE2" s="216"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -43857,31 +43860,31 @@
         <v>20.923299999999998</v>
       </c>
       <c r="O3" s="82"/>
-      <c r="P3" s="203" t="s">
+      <c r="P3" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="203"/>
-      <c r="R3" s="203"/>
-      <c r="S3" s="203" t="s">
+      <c r="Q3" s="211"/>
+      <c r="R3" s="211"/>
+      <c r="S3" s="211" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="203"/>
-      <c r="U3" s="203"/>
-      <c r="V3" s="203" t="s">
+      <c r="T3" s="211"/>
+      <c r="U3" s="211"/>
+      <c r="V3" s="211" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="203"/>
-      <c r="X3" s="203"/>
-      <c r="Y3" s="203" t="s">
+      <c r="W3" s="211"/>
+      <c r="X3" s="211"/>
+      <c r="Y3" s="211" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="203"/>
-      <c r="AA3" s="203"/>
-      <c r="AB3" s="203" t="s">
+      <c r="Z3" s="211"/>
+      <c r="AA3" s="211"/>
+      <c r="AB3" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="AC3" s="203"/>
-      <c r="AD3" s="203"/>
+      <c r="AC3" s="211"/>
+      <c r="AD3" s="211"/>
       <c r="AE3" s="10"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -44295,14 +44298,14 @@
       <c r="I8" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="219" t="s">
+      <c r="J8" s="221" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="219"/>
-      <c r="L8" s="215" t="s">
+      <c r="K8" s="221"/>
+      <c r="L8" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="215"/>
+      <c r="M8" s="222"/>
       <c r="O8" s="114" t="s">
         <v>53</v>
       </c>
@@ -44911,25 +44914,25 @@
       <c r="I15" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="216" t="s">
+      <c r="O15" s="219" t="s">
         <v>33</v>
       </c>
-      <c r="P15" s="216"/>
-      <c r="Q15" s="216"/>
-      <c r="R15" s="216"/>
-      <c r="S15" s="216"/>
-      <c r="T15" s="216"/>
-      <c r="U15" s="216"/>
-      <c r="V15" s="216"/>
-      <c r="W15" s="216"/>
-      <c r="X15" s="216"/>
-      <c r="Y15" s="216"/>
-      <c r="Z15" s="216"/>
-      <c r="AA15" s="216"/>
-      <c r="AB15" s="216"/>
-      <c r="AC15" s="216"/>
-      <c r="AD15" s="216"/>
-      <c r="AE15" s="216"/>
+      <c r="P15" s="219"/>
+      <c r="Q15" s="219"/>
+      <c r="R15" s="219"/>
+      <c r="S15" s="219"/>
+      <c r="T15" s="219"/>
+      <c r="U15" s="219"/>
+      <c r="V15" s="219"/>
+      <c r="W15" s="219"/>
+      <c r="X15" s="219"/>
+      <c r="Y15" s="219"/>
+      <c r="Z15" s="219"/>
+      <c r="AA15" s="219"/>
+      <c r="AB15" s="219"/>
+      <c r="AC15" s="219"/>
+      <c r="AD15" s="219"/>
+      <c r="AE15" s="219"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -44957,31 +44960,31 @@
         <v>72</v>
       </c>
       <c r="O16" s="1"/>
-      <c r="P16" s="216" t="s">
+      <c r="P16" s="219" t="s">
         <v>34</v>
       </c>
-      <c r="Q16" s="216"/>
-      <c r="R16" s="216"/>
-      <c r="S16" s="216" t="s">
+      <c r="Q16" s="219"/>
+      <c r="R16" s="219"/>
+      <c r="S16" s="219" t="s">
         <v>35</v>
       </c>
-      <c r="T16" s="216"/>
-      <c r="U16" s="216"/>
-      <c r="V16" s="216" t="s">
+      <c r="T16" s="219"/>
+      <c r="U16" s="219"/>
+      <c r="V16" s="219" t="s">
         <v>36</v>
       </c>
-      <c r="W16" s="216"/>
-      <c r="X16" s="216"/>
-      <c r="Y16" s="216" t="s">
+      <c r="W16" s="219"/>
+      <c r="X16" s="219"/>
+      <c r="Y16" s="219" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="216"/>
-      <c r="AA16" s="216"/>
-      <c r="AB16" s="216" t="s">
+      <c r="Z16" s="219"/>
+      <c r="AA16" s="219"/>
+      <c r="AB16" s="219" t="s">
         <v>55</v>
       </c>
-      <c r="AC16" s="216"/>
-      <c r="AD16" s="216"/>
+      <c r="AC16" s="219"/>
+      <c r="AD16" s="219"/>
       <c r="AE16" s="1"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -45758,10 +45761,10 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="216" t="s">
+      <c r="B28" s="219" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="216"/>
+      <c r="C28" s="219"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B29" s="116" t="s">
@@ -46130,25 +46133,25 @@
       <c r="G45" s="125">
         <v>0.46912291153627583</v>
       </c>
-      <c r="O45" s="209" t="s">
+      <c r="O45" s="212" t="s">
         <v>57</v>
       </c>
-      <c r="P45" s="210"/>
-      <c r="Q45" s="210"/>
-      <c r="R45" s="210"/>
-      <c r="S45" s="210"/>
-      <c r="T45" s="210"/>
-      <c r="U45" s="210"/>
-      <c r="V45" s="210"/>
-      <c r="W45" s="210"/>
-      <c r="X45" s="210"/>
-      <c r="Y45" s="210"/>
-      <c r="Z45" s="210"/>
-      <c r="AA45" s="210"/>
-      <c r="AB45" s="210"/>
-      <c r="AC45" s="210"/>
-      <c r="AD45" s="210"/>
-      <c r="AE45" s="211"/>
+      <c r="P45" s="213"/>
+      <c r="Q45" s="213"/>
+      <c r="R45" s="213"/>
+      <c r="S45" s="213"/>
+      <c r="T45" s="213"/>
+      <c r="U45" s="213"/>
+      <c r="V45" s="213"/>
+      <c r="W45" s="213"/>
+      <c r="X45" s="213"/>
+      <c r="Y45" s="213"/>
+      <c r="Z45" s="213"/>
+      <c r="AA45" s="213"/>
+      <c r="AB45" s="213"/>
+      <c r="AC45" s="213"/>
+      <c r="AD45" s="213"/>
+      <c r="AE45" s="214"/>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -46172,25 +46175,25 @@
       <c r="G46" s="121">
         <v>0.28048507488986779</v>
       </c>
-      <c r="O46" s="207" t="s">
+      <c r="O46" s="215" t="s">
         <v>51</v>
       </c>
-      <c r="P46" s="208"/>
-      <c r="Q46" s="208"/>
-      <c r="R46" s="208"/>
-      <c r="S46" s="208"/>
-      <c r="T46" s="208"/>
-      <c r="U46" s="208"/>
-      <c r="V46" s="208"/>
-      <c r="W46" s="208"/>
-      <c r="X46" s="208"/>
-      <c r="Y46" s="208"/>
-      <c r="Z46" s="208"/>
-      <c r="AA46" s="208"/>
-      <c r="AB46" s="208"/>
-      <c r="AC46" s="208"/>
-      <c r="AD46" s="208"/>
-      <c r="AE46" s="208"/>
+      <c r="P46" s="216"/>
+      <c r="Q46" s="216"/>
+      <c r="R46" s="216"/>
+      <c r="S46" s="216"/>
+      <c r="T46" s="216"/>
+      <c r="U46" s="216"/>
+      <c r="V46" s="216"/>
+      <c r="W46" s="216"/>
+      <c r="X46" s="216"/>
+      <c r="Y46" s="216"/>
+      <c r="Z46" s="216"/>
+      <c r="AA46" s="216"/>
+      <c r="AB46" s="216"/>
+      <c r="AC46" s="216"/>
+      <c r="AD46" s="216"/>
+      <c r="AE46" s="216"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -46215,31 +46218,31 @@
         <v>0.29737257882304624</v>
       </c>
       <c r="O47" s="82"/>
-      <c r="P47" s="203" t="s">
+      <c r="P47" s="211" t="s">
         <v>34</v>
       </c>
-      <c r="Q47" s="203"/>
-      <c r="R47" s="203"/>
-      <c r="S47" s="203" t="s">
+      <c r="Q47" s="211"/>
+      <c r="R47" s="211"/>
+      <c r="S47" s="211" t="s">
         <v>35</v>
       </c>
-      <c r="T47" s="203"/>
-      <c r="U47" s="203"/>
-      <c r="V47" s="203" t="s">
+      <c r="T47" s="211"/>
+      <c r="U47" s="211"/>
+      <c r="V47" s="211" t="s">
         <v>36</v>
       </c>
-      <c r="W47" s="203"/>
-      <c r="X47" s="203"/>
-      <c r="Y47" s="203" t="s">
+      <c r="W47" s="211"/>
+      <c r="X47" s="211"/>
+      <c r="Y47" s="211" t="s">
         <v>37</v>
       </c>
-      <c r="Z47" s="203"/>
-      <c r="AA47" s="203"/>
-      <c r="AB47" s="203" t="s">
+      <c r="Z47" s="211"/>
+      <c r="AA47" s="211"/>
+      <c r="AB47" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="AC47" s="203"/>
-      <c r="AD47" s="203"/>
+      <c r="AC47" s="211"/>
+      <c r="AD47" s="211"/>
       <c r="AE47" s="10"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
@@ -46450,26 +46453,26 @@
       </c>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A51" s="219" t="s">
+      <c r="A51" s="221" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="219"/>
-      <c r="C51" s="219"/>
-      <c r="D51" s="219"/>
-      <c r="E51" s="219"/>
-      <c r="F51" s="219"/>
-      <c r="G51" s="219"/>
+      <c r="B51" s="221"/>
+      <c r="C51" s="221"/>
+      <c r="D51" s="221"/>
+      <c r="E51" s="221"/>
+      <c r="F51" s="221"/>
+      <c r="G51" s="221"/>
       <c r="I51" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="J51" s="219" t="s">
+      <c r="J51" s="221" t="s">
         <v>57</v>
       </c>
-      <c r="K51" s="219"/>
-      <c r="L51" s="215" t="s">
+      <c r="K51" s="221"/>
+      <c r="L51" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="M51" s="215"/>
+      <c r="M51" s="222"/>
       <c r="O51" s="97" t="s">
         <v>44</v>
       </c>
@@ -46526,10 +46529,10 @@
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B52" s="216" t="s">
+      <c r="B52" s="219" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="216"/>
+      <c r="C52" s="219"/>
       <c r="I52" s="135" t="s">
         <v>65</v>
       </c>
@@ -47084,14 +47087,14 @@
       <c r="I58" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="J58" s="219" t="s">
+      <c r="J58" s="221" t="s">
         <v>57</v>
       </c>
-      <c r="K58" s="219"/>
-      <c r="L58" s="215" t="s">
+      <c r="K58" s="221"/>
+      <c r="L58" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="M58" s="215"/>
+      <c r="M58" s="222"/>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="152" t="s">
@@ -47130,25 +47133,25 @@
       <c r="M59" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="O59" s="204" t="s">
+      <c r="O59" s="205" t="s">
         <v>33</v>
       </c>
-      <c r="P59" s="205"/>
-      <c r="Q59" s="205"/>
-      <c r="R59" s="205"/>
-      <c r="S59" s="205"/>
-      <c r="T59" s="205"/>
-      <c r="U59" s="205"/>
-      <c r="V59" s="205"/>
-      <c r="W59" s="205"/>
-      <c r="X59" s="205"/>
-      <c r="Y59" s="205"/>
-      <c r="Z59" s="205"/>
-      <c r="AA59" s="205"/>
-      <c r="AB59" s="205"/>
-      <c r="AC59" s="205"/>
-      <c r="AD59" s="205"/>
-      <c r="AE59" s="206"/>
+      <c r="P59" s="206"/>
+      <c r="Q59" s="206"/>
+      <c r="R59" s="206"/>
+      <c r="S59" s="206"/>
+      <c r="T59" s="206"/>
+      <c r="U59" s="206"/>
+      <c r="V59" s="206"/>
+      <c r="W59" s="206"/>
+      <c r="X59" s="206"/>
+      <c r="Y59" s="206"/>
+      <c r="Z59" s="206"/>
+      <c r="AA59" s="206"/>
+      <c r="AB59" s="206"/>
+      <c r="AC59" s="206"/>
+      <c r="AD59" s="206"/>
+      <c r="AE59" s="207"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="153" t="s">
@@ -47192,31 +47195,31 @@
         <v>0.98799999999999999</v>
       </c>
       <c r="O60" s="82"/>
-      <c r="P60" s="212" t="s">
+      <c r="P60" s="208" t="s">
         <v>34</v>
       </c>
-      <c r="Q60" s="213"/>
-      <c r="R60" s="214"/>
-      <c r="S60" s="212" t="s">
+      <c r="Q60" s="209"/>
+      <c r="R60" s="210"/>
+      <c r="S60" s="208" t="s">
         <v>35</v>
       </c>
-      <c r="T60" s="213"/>
-      <c r="U60" s="214"/>
-      <c r="V60" s="212" t="s">
+      <c r="T60" s="209"/>
+      <c r="U60" s="210"/>
+      <c r="V60" s="208" t="s">
         <v>36</v>
       </c>
-      <c r="W60" s="213"/>
-      <c r="X60" s="214"/>
-      <c r="Y60" s="212" t="s">
+      <c r="W60" s="209"/>
+      <c r="X60" s="210"/>
+      <c r="Y60" s="208" t="s">
         <v>37</v>
       </c>
-      <c r="Z60" s="213"/>
-      <c r="AA60" s="214"/>
-      <c r="AB60" s="203" t="s">
+      <c r="Z60" s="209"/>
+      <c r="AA60" s="210"/>
+      <c r="AB60" s="211" t="s">
         <v>55</v>
       </c>
-      <c r="AC60" s="203"/>
-      <c r="AD60" s="203"/>
+      <c r="AC60" s="211"/>
+      <c r="AD60" s="211"/>
       <c r="AE60" s="1"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
@@ -48730,14 +48733,27 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="O59:AE59"/>
-    <mergeCell ref="P60:R60"/>
-    <mergeCell ref="S60:U60"/>
-    <mergeCell ref="V60:X60"/>
-    <mergeCell ref="Y60:AA60"/>
-    <mergeCell ref="AB60:AD60"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="AB16:AD16"/>
+    <mergeCell ref="O15:AE15"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="O1:AE1"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B82:C82"/>
     <mergeCell ref="O45:AE45"/>
@@ -48752,27 +48768,14 @@
     <mergeCell ref="L51:M51"/>
     <mergeCell ref="J58:K58"/>
     <mergeCell ref="L58:M58"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="AB16:AD16"/>
-    <mergeCell ref="O15:AE15"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="O1:AE1"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="O59:AE59"/>
+    <mergeCell ref="P60:R60"/>
+    <mergeCell ref="S60:U60"/>
+    <mergeCell ref="V60:X60"/>
+    <mergeCell ref="Y60:AA60"/>
+    <mergeCell ref="AB60:AD60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -48783,8 +48786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74D7792-97E4-49F1-9599-DBFEA25C1ED6}">
   <dimension ref="A1:AD108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AD70" sqref="AD70"/>
+    <sheetView tabSelected="1" topLeftCell="X19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AL32" sqref="AL32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48812,18 +48815,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="219" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="216"/>
-      <c r="J1" s="216" t="s">
+      <c r="C1" s="219"/>
+      <c r="J1" s="219" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="216"/>
-      <c r="R1" s="222" t="s">
+      <c r="K1" s="219"/>
+      <c r="R1" s="224" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="222"/>
+      <c r="S1" s="224"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -48863,26 +48866,26 @@
       <c r="O2" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="221" t="s">
+      <c r="R2" s="223" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="221"/>
-      <c r="T2" s="221" t="s">
+      <c r="S2" s="223"/>
+      <c r="T2" s="223" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="221"/>
-      <c r="V2" s="221" t="s">
+      <c r="U2" s="223"/>
+      <c r="V2" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="W2" s="221"/>
-      <c r="X2" s="221" t="s">
+      <c r="W2" s="223"/>
+      <c r="X2" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="Y2" s="221"/>
-      <c r="Z2" s="221" t="s">
+      <c r="Y2" s="223"/>
+      <c r="Z2" s="223" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" s="221"/>
+      <c r="AA2" s="223"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -48962,7 +48965,7 @@
       <c r="AA3" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="223" t="s">
+      <c r="AC3" s="202" t="s">
         <v>106</v>
       </c>
     </row>
@@ -49719,10 +49722,10 @@
         <f t="shared" si="13"/>
         <v>8.5902314408056568E-2</v>
       </c>
-      <c r="R12" s="222" t="s">
+      <c r="R12" s="224" t="s">
         <v>89</v>
       </c>
-      <c r="S12" s="222"/>
+      <c r="S12" s="224"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -49772,26 +49775,26 @@
         <f t="shared" si="14"/>
         <v>0.19838337462369771</v>
       </c>
-      <c r="R13" s="221" t="s">
+      <c r="R13" s="223" t="s">
         <v>86</v>
       </c>
-      <c r="S13" s="221"/>
-      <c r="T13" s="221" t="s">
+      <c r="S13" s="223"/>
+      <c r="T13" s="223" t="s">
         <v>98</v>
       </c>
-      <c r="U13" s="221"/>
-      <c r="V13" s="221" t="s">
+      <c r="U13" s="223"/>
+      <c r="V13" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="W13" s="221"/>
-      <c r="X13" s="221" t="s">
+      <c r="W13" s="223"/>
+      <c r="X13" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="Y13" s="221"/>
-      <c r="Z13" s="221" t="s">
+      <c r="Y13" s="223"/>
+      <c r="Z13" s="223" t="s">
         <v>97</v>
       </c>
-      <c r="AA13" s="221"/>
+      <c r="AA13" s="223"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B14" s="217" t="s">
@@ -50327,10 +50330,10 @@
       <c r="G20" s="33">
         <v>0.14591900352662099</v>
       </c>
-      <c r="J20" s="216" t="s">
+      <c r="J20" s="219" t="s">
         <v>92</v>
       </c>
-      <c r="K20" s="216"/>
+      <c r="K20" s="219"/>
       <c r="Q20" s="8" t="s">
         <v>11</v>
       </c>
@@ -50694,10 +50697,10 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="216" t="s">
+      <c r="B28" s="219" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="216"/>
+      <c r="C28" s="219"/>
       <c r="J28" s="217" t="s">
         <v>93</v>
       </c>
@@ -51175,10 +51178,10 @@
       <c r="G43" s="35">
         <v>0.3607486615802406</v>
       </c>
-      <c r="R43" s="222" t="s">
+      <c r="R43" s="224" t="s">
         <v>104</v>
       </c>
-      <c r="S43" s="222"/>
+      <c r="S43" s="224"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -51202,26 +51205,26 @@
       <c r="G44" s="35">
         <v>0.23478451896362351</v>
       </c>
-      <c r="R44" s="221" t="s">
+      <c r="R44" s="223" t="s">
         <v>86</v>
       </c>
-      <c r="S44" s="221"/>
-      <c r="T44" s="221" t="s">
+      <c r="S44" s="223"/>
+      <c r="T44" s="223" t="s">
         <v>94</v>
       </c>
-      <c r="U44" s="221"/>
-      <c r="V44" s="221" t="s">
+      <c r="U44" s="223"/>
+      <c r="V44" s="223" t="s">
         <v>95</v>
       </c>
-      <c r="W44" s="221"/>
-      <c r="X44" s="221" t="s">
+      <c r="W44" s="223"/>
+      <c r="X44" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="Y44" s="221"/>
-      <c r="Z44" s="221" t="s">
+      <c r="Y44" s="223"/>
+      <c r="Z44" s="223" t="s">
         <v>97</v>
       </c>
-      <c r="AA44" s="221"/>
+      <c r="AA44" s="223"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -51275,10 +51278,10 @@
       <c r="AA45" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="AC45" s="223" t="s">
+      <c r="AC45" s="202" t="s">
         <v>108</v>
       </c>
-      <c r="AD45" s="223" t="s">
+      <c r="AD45" s="202" t="s">
         <v>109</v>
       </c>
     </row>
@@ -51658,15 +51661,15 @@
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A51" s="219" t="s">
+      <c r="A51" s="221" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="219"/>
-      <c r="C51" s="219"/>
-      <c r="D51" s="219"/>
-      <c r="E51" s="219"/>
-      <c r="F51" s="219"/>
-      <c r="G51" s="219"/>
+      <c r="B51" s="221"/>
+      <c r="C51" s="221"/>
+      <c r="D51" s="221"/>
+      <c r="E51" s="221"/>
+      <c r="F51" s="221"/>
+      <c r="G51" s="221"/>
       <c r="Q51" s="7" t="s">
         <v>83</v>
       </c>
@@ -51721,10 +51724,10 @@
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B52" s="216" t="s">
+      <c r="B52" s="219" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="216"/>
+      <c r="C52" s="219"/>
       <c r="Q52" s="8" t="s">
         <v>84</v>
       </c>
@@ -51821,11 +51824,11 @@
       <c r="G54" s="36">
         <v>0.16000831182380926</v>
       </c>
-      <c r="R54" s="222" t="s">
+      <c r="R54" s="224" t="s">
         <v>105</v>
       </c>
-      <c r="S54" s="222"/>
-      <c r="AD54" s="35"/>
+      <c r="S54" s="224"/>
+      <c r="AD54" s="225"/>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" s="150" t="s">
@@ -51849,26 +51852,26 @@
       <c r="G55" s="36">
         <v>0.12962202535912964</v>
       </c>
-      <c r="R55" s="221" t="s">
+      <c r="R55" s="223" t="s">
         <v>86</v>
       </c>
-      <c r="S55" s="221"/>
-      <c r="T55" s="221" t="s">
+      <c r="S55" s="223"/>
+      <c r="T55" s="223" t="s">
         <v>98</v>
       </c>
-      <c r="U55" s="221"/>
-      <c r="V55" s="221" t="s">
+      <c r="U55" s="223"/>
+      <c r="V55" s="223" t="s">
         <v>99</v>
       </c>
-      <c r="W55" s="221"/>
-      <c r="X55" s="221" t="s">
+      <c r="W55" s="223"/>
+      <c r="X55" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="Y55" s="221"/>
-      <c r="Z55" s="221" t="s">
+      <c r="Y55" s="223"/>
+      <c r="Z55" s="223" t="s">
         <v>97</v>
       </c>
-      <c r="AA55" s="221"/>
+      <c r="AA55" s="223"/>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="151" t="s">
@@ -51922,7 +51925,7 @@
       <c r="AA56" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="AC56" s="223" t="s">
+      <c r="AC56" s="202" t="s">
         <v>107</v>
       </c>
     </row>
@@ -51948,10 +51951,10 @@
       <c r="G57" s="36">
         <v>0.12090681526084991</v>
       </c>
-      <c r="J57" s="216" t="s">
+      <c r="J57" s="219" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="216"/>
+      <c r="K57" s="219"/>
       <c r="Q57" s="2" t="s">
         <v>78</v>
       </c>
@@ -52091,7 +52094,7 @@
       <c r="AB58" s="83">
         <v>-0.32001589401318453</v>
       </c>
-      <c r="AC58" s="224">
+      <c r="AC58" s="203">
         <v>-0.32483084673747942</v>
       </c>
       <c r="AD58" s="31">
@@ -52551,6 +52554,7 @@
         <v>0.22393563169580205</v>
       </c>
       <c r="AC63" s="119"/>
+      <c r="AD63" s="35"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="155" t="s">
@@ -52600,7 +52604,6 @@
         <f t="shared" si="56"/>
         <v>5.3915099455572491E-2</v>
       </c>
-      <c r="AD64" s="35"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="155" t="s">
@@ -53088,10 +53091,10 @@
       <c r="G77" s="72">
         <v>8.7751258894774364E-2</v>
       </c>
-      <c r="J77" s="216" t="s">
+      <c r="J77" s="219" t="s">
         <v>102</v>
       </c>
-      <c r="K77" s="216"/>
+      <c r="K77" s="219"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="154" t="s">
@@ -54100,6 +54103,33 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="T55:U55"/>
+    <mergeCell ref="V55:W55"/>
+    <mergeCell ref="X55:Y55"/>
+    <mergeCell ref="Z55:AA55"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="J77:K77"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="R43:S43"/>
+    <mergeCell ref="R44:S44"/>
+    <mergeCell ref="R54:S54"/>
+    <mergeCell ref="R55:S55"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="T44:U44"/>
+    <mergeCell ref="V44:W44"/>
+    <mergeCell ref="X44:Y44"/>
+    <mergeCell ref="Z44:AA44"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B14:C14"/>
@@ -54114,33 +54144,6 @@
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="T44:U44"/>
-    <mergeCell ref="V44:W44"/>
-    <mergeCell ref="X44:Y44"/>
-    <mergeCell ref="Z44:AA44"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:U13"/>
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="X13:Y13"/>
-    <mergeCell ref="Z13:AA13"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="J77:K77"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="R43:S43"/>
-    <mergeCell ref="R44:S44"/>
-    <mergeCell ref="R54:S54"/>
-    <mergeCell ref="R55:S55"/>
-    <mergeCell ref="T55:U55"/>
-    <mergeCell ref="V55:W55"/>
-    <mergeCell ref="X55:Y55"/>
-    <mergeCell ref="Z55:AA55"/>
-    <mergeCell ref="J57:K57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>